<commit_message>
Additional changes on VIS portal
</commit_message>
<xml_diff>
--- a/Data/VanguardConfig.xlsx
+++ b/Data/VanguardConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\603213\Documents\UiPath\Vangaurd\RoboticEnterpriseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42907FA3-93F0-4E7C-8E56-D52F89D42379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384D8D3B-460D-486C-99FA-25DADCAD8D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1005,6 +1005,9 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
         <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -2436,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>